<commit_message>
fixed mistake in pixel measurement
</commit_message>
<xml_diff>
--- a/Ex-3/focal_length.xlsx
+++ b/Ex-3/focal_length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prog\uni\REX\REX\Ex-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ED48D73-64F4-4EE1-8F66-A19D9FB1E905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E021ACBE-D7F8-4A6E-AE25-D1AB50B027BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{929DEB90-BB08-49B5-B1F5-EDBB5F6E4B0C}"/>
   </bookViews>
@@ -429,7 +429,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,11 +515,11 @@
         <v>3300</v>
       </c>
       <c r="B7">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>1524.8275862068965</v>
+        <v>1251.7241379310344</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -584,7 +584,7 @@
       </c>
       <c r="C14" s="1">
         <f>AVERAGE(C2:C11)</f>
-        <v>1283.9999999999998</v>
+        <v>1256.6896551724135</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -595,7 +595,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C16" s="1">
         <f>_xlfn.STDEV.P(C2:C11)</f>
-        <v>86.571806984525821</v>
+        <v>32.453094295764785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>